<commit_message>
added EF shell. Initial parse of correctly formatted product spreadsheet
</commit_message>
<xml_diff>
--- a/TNS.Tests/bin/Debug/Book1.xlsx
+++ b/TNS.Tests/bin/Debug/Book1.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>score 1</t>
   </si>
@@ -361,7 +360,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -374,7 +373,7 @@
         <v>12</v>
       </c>
       <c r="C1">
-        <v>999</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -385,7 +384,7 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>888</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -393,10 +392,10 @@
         <v>2</v>
       </c>
       <c r="B3">
+        <v>35</v>
+      </c>
+      <c r="C3">
         <v>21</v>
-      </c>
-      <c r="C3">
-        <v>777</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -404,57 +403,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4">
-        <v>666</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>66</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>